<commit_message>
Observe the provide data
</commit_message>
<xml_diff>
--- a/PM25_Coding/Data_cleaning/PM2.5/PM2.5_2017_.xlsx
+++ b/PM25_Coding/Data_cleaning/PM2.5/PM2.5_2017_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\DataMining_PM2_5\PM25_Coding\Data_cleaning\PM2.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC06F43-0500-482E-804A-E58A14DC437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E123B5A9-2CCB-4192-A759-627E1FCA6A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,9 +226,6 @@
     <t xml:space="preserve"> ต.ทรงคนอง  อ.พระประแดง  จ.สมุทรปราการ</t>
   </si>
   <si>
-    <t xml:space="preserve"> ต.หน้าพระลาน อ.เฉลิมพระเกียรติ จ.สระบุรี </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ต.หน้าเมือง อ.เมือง จ.ราชบุรี</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>รหัสสถานี</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ต.หน้าพระลาน อ.เฉลิมพระเกียรติ จ.สระบุรี</t>
   </si>
 </sst>
 </file>
@@ -31312,7 +31312,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -31325,7 +31325,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>28</v>
@@ -31438,7 +31438,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>39</v>
@@ -31449,7 +31449,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>40</v>
@@ -31460,7 +31460,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>41</v>
@@ -31471,7 +31471,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>44</v>
@@ -31482,7 +31482,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>45</v>
@@ -31493,7 +31493,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>47</v>
@@ -31504,7 +31504,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>48</v>
@@ -31515,7 +31515,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>49</v>
@@ -31526,7 +31526,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>52</v>
@@ -31537,7 +31537,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>43</v>
@@ -31548,7 +31548,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>53</v>
@@ -31559,7 +31559,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>54</v>
@@ -31570,7 +31570,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>50</v>
@@ -31582,7 +31582,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>51</v>
@@ -31594,7 +31594,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>46</v>
@@ -31606,7 +31606,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>42</v>
@@ -31617,7 +31617,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>55</v>

</xml_diff>